<commit_message>
Change shop (add fields + change initial shop list)
</commit_message>
<xml_diff>
--- a/xlsforms/shop.xlsx
+++ b/xlsforms/shop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -45,10 +45,37 @@
     <t xml:space="preserve">Name </t>
   </si>
   <si>
-    <t xml:space="preserve">adress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adress</t>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main product(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website</t>
   </si>
   <si>
     <t xml:space="preserve">select_one location_choices</t>
@@ -262,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,7 +318,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,10 +423,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ25"/>
+  <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -440,101 +475,162 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G4" s="4"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="5" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G5" s="4"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="G6" s="9"/>
+      <c r="AMJ6" s="9"/>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="G7" s="9"/>
+      <c r="AMJ7" s="9"/>
+    </row>
+    <row r="8" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="G8" s="9"/>
+      <c r="AMJ8" s="9"/>
+    </row>
+    <row r="9" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="0"/>
-    </row>
-    <row r="10" s="7" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G9" s="9"/>
+      <c r="AMJ9" s="9"/>
+    </row>
+    <row r="10" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G10" s="4"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="0"/>
+    </row>
+    <row r="16" s="8" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="4"/>
+      <c r="AMJ16" s="0"/>
+    </row>
     <row r="17" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -564,6 +660,12 @@
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -588,57 +690,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="81.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="8" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="81.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="10" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D4" s="0"/>
     </row>
@@ -675,7 +777,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -690,34 +792,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>34</v>
+      <c r="A1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="11" t="n">
+      <c r="A2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>